<commit_message>
add Dirt class. New river design
</commit_message>
<xml_diff>
--- a/Game/River designs.xlsx
+++ b/Game/River designs.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="14360" yWindow="460" windowWidth="18580" windowHeight="14320" tabRatio="500"/>
+    <workbookView xWindow="22660" yWindow="460" windowWidth="28540" windowHeight="27040" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="River1 20x20" sheetId="1" r:id="rId1"/>
+    <sheet name="River2 30x30" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -39,7 +40,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -47,8 +48,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="4" tint="0.39997558519241921"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -79,6 +87,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -227,7 +241,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -244,12 +258,20 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF9BC2E6"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -523,8 +545,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:U21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1111,4 +1133,1174 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:AF41"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="AI14" sqref="AI14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="34" width="4.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:32" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="2:32" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="3" spans="2:32" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <v>3</v>
+      </c>
+      <c r="G3">
+        <v>4</v>
+      </c>
+      <c r="H3">
+        <v>5</v>
+      </c>
+      <c r="I3">
+        <v>6</v>
+      </c>
+      <c r="J3">
+        <v>7</v>
+      </c>
+      <c r="K3">
+        <v>8</v>
+      </c>
+      <c r="L3">
+        <v>9</v>
+      </c>
+      <c r="M3">
+        <v>10</v>
+      </c>
+      <c r="N3">
+        <v>11</v>
+      </c>
+      <c r="O3">
+        <v>12</v>
+      </c>
+      <c r="P3">
+        <v>13</v>
+      </c>
+      <c r="Q3">
+        <v>14</v>
+      </c>
+      <c r="R3">
+        <v>15</v>
+      </c>
+      <c r="S3">
+        <v>16</v>
+      </c>
+      <c r="T3">
+        <v>17</v>
+      </c>
+      <c r="U3">
+        <v>18</v>
+      </c>
+      <c r="V3">
+        <v>19</v>
+      </c>
+      <c r="W3">
+        <v>20</v>
+      </c>
+      <c r="X3">
+        <v>21</v>
+      </c>
+      <c r="Y3">
+        <v>22</v>
+      </c>
+      <c r="Z3">
+        <v>23</v>
+      </c>
+      <c r="AA3">
+        <v>24</v>
+      </c>
+      <c r="AB3">
+        <v>25</v>
+      </c>
+      <c r="AC3">
+        <v>26</v>
+      </c>
+      <c r="AD3">
+        <v>27</v>
+      </c>
+      <c r="AE3">
+        <v>28</v>
+      </c>
+      <c r="AF3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="2:32" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="5"/>
+      <c r="O4" s="5"/>
+      <c r="P4" s="5"/>
+      <c r="Q4" s="5"/>
+      <c r="R4" s="5"/>
+      <c r="S4" s="5"/>
+      <c r="T4" s="5"/>
+      <c r="U4" s="5"/>
+      <c r="V4" s="5"/>
+      <c r="W4" s="5"/>
+      <c r="X4" s="5"/>
+      <c r="Y4" s="5"/>
+      <c r="Z4" s="5"/>
+      <c r="AA4" s="5"/>
+      <c r="AB4" s="5"/>
+      <c r="AC4" s="5"/>
+      <c r="AD4" s="5"/>
+      <c r="AE4" s="5"/>
+      <c r="AF4" s="5"/>
+    </row>
+    <row r="5" spans="2:32" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="5"/>
+      <c r="O5" s="5"/>
+      <c r="P5" s="5"/>
+      <c r="Q5" s="5"/>
+      <c r="R5" s="5"/>
+      <c r="S5" s="5"/>
+      <c r="T5" s="5"/>
+      <c r="U5" s="5"/>
+      <c r="V5" s="5"/>
+      <c r="W5" s="5"/>
+      <c r="X5" s="5"/>
+      <c r="Y5" s="5"/>
+      <c r="Z5" s="5"/>
+      <c r="AA5" s="5"/>
+      <c r="AB5" s="5"/>
+      <c r="AC5" s="5"/>
+      <c r="AD5" s="5"/>
+      <c r="AE5" s="5"/>
+      <c r="AF5" s="5"/>
+    </row>
+    <row r="6" spans="2:32" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5"/>
+      <c r="N6" s="5"/>
+      <c r="O6" s="5"/>
+      <c r="P6" s="5"/>
+      <c r="Q6" s="5"/>
+      <c r="R6" s="5"/>
+      <c r="S6" s="5"/>
+      <c r="T6" s="5"/>
+      <c r="U6" s="5"/>
+      <c r="V6" s="5"/>
+      <c r="W6" s="5"/>
+      <c r="X6" s="5"/>
+      <c r="Y6" s="5"/>
+      <c r="Z6" s="5"/>
+      <c r="AA6" s="5"/>
+      <c r="AB6" s="5"/>
+      <c r="AC6" s="5"/>
+      <c r="AD6" s="5"/>
+      <c r="AE6" s="5"/>
+      <c r="AF6" s="5"/>
+    </row>
+    <row r="7" spans="2:32" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7">
+        <v>3</v>
+      </c>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="5"/>
+      <c r="N7" s="5"/>
+      <c r="O7" s="5"/>
+      <c r="P7" s="5"/>
+      <c r="Q7" s="5"/>
+      <c r="R7" s="5"/>
+      <c r="S7" s="5"/>
+      <c r="T7" s="5"/>
+      <c r="U7" s="5"/>
+      <c r="V7" s="5"/>
+      <c r="W7" s="5"/>
+      <c r="X7" s="5"/>
+      <c r="Y7" s="5"/>
+      <c r="Z7" s="5"/>
+      <c r="AA7" s="5"/>
+      <c r="AB7" s="5"/>
+      <c r="AC7" s="5"/>
+      <c r="AD7" s="5"/>
+      <c r="AE7" s="5"/>
+      <c r="AF7" s="5"/>
+    </row>
+    <row r="8" spans="2:32" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8">
+        <v>4</v>
+      </c>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="18"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="5"/>
+      <c r="N8" s="5"/>
+      <c r="O8" s="5"/>
+      <c r="P8" s="5"/>
+      <c r="Q8" s="5"/>
+      <c r="R8" s="5"/>
+      <c r="S8" s="5"/>
+      <c r="T8" s="18"/>
+      <c r="U8" s="5"/>
+      <c r="V8" s="5"/>
+      <c r="W8" s="5"/>
+      <c r="X8" s="5"/>
+      <c r="Y8" s="5"/>
+      <c r="Z8" s="5"/>
+      <c r="AA8" s="5"/>
+      <c r="AB8" s="5"/>
+      <c r="AC8" s="5"/>
+      <c r="AD8" s="5"/>
+      <c r="AE8" s="5"/>
+      <c r="AF8" s="5"/>
+    </row>
+    <row r="9" spans="2:32" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B9">
+        <v>5</v>
+      </c>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="18"/>
+      <c r="I9" s="18"/>
+      <c r="J9" s="18"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
+      <c r="M9" s="5"/>
+      <c r="N9" s="5"/>
+      <c r="O9" s="5"/>
+      <c r="P9" s="5"/>
+      <c r="Q9" s="5"/>
+      <c r="R9" s="5"/>
+      <c r="S9" s="18"/>
+      <c r="T9" s="5"/>
+      <c r="U9" s="5"/>
+      <c r="V9" s="5"/>
+      <c r="W9" s="5"/>
+      <c r="X9" s="5"/>
+      <c r="Y9" s="5"/>
+      <c r="Z9" s="5"/>
+      <c r="AA9" s="5"/>
+      <c r="AB9" s="5"/>
+      <c r="AC9" s="5"/>
+      <c r="AD9" s="5"/>
+      <c r="AE9" s="5"/>
+      <c r="AF9" s="5"/>
+    </row>
+    <row r="10" spans="2:32" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B10">
+        <v>6</v>
+      </c>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="18"/>
+      <c r="K10" s="18"/>
+      <c r="L10" s="18"/>
+      <c r="M10" s="18"/>
+      <c r="N10" s="18"/>
+      <c r="O10" s="5"/>
+      <c r="P10" s="5"/>
+      <c r="Q10" s="5"/>
+      <c r="R10" s="18"/>
+      <c r="S10" s="5"/>
+      <c r="T10" s="5"/>
+      <c r="U10" s="5"/>
+      <c r="V10" s="5"/>
+      <c r="W10" s="5"/>
+      <c r="X10" s="5"/>
+      <c r="Y10" s="5"/>
+      <c r="Z10" s="18"/>
+      <c r="AA10" s="5"/>
+      <c r="AB10" s="5"/>
+      <c r="AC10" s="5"/>
+      <c r="AD10" s="5"/>
+      <c r="AE10" s="5"/>
+      <c r="AF10" s="5"/>
+    </row>
+    <row r="11" spans="2:32" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11">
+        <v>7</v>
+      </c>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="18"/>
+      <c r="N11" s="18"/>
+      <c r="O11" s="18"/>
+      <c r="P11" s="5"/>
+      <c r="Q11" s="18"/>
+      <c r="R11" s="5"/>
+      <c r="S11" s="5"/>
+      <c r="T11" s="5"/>
+      <c r="U11" s="5"/>
+      <c r="V11" s="5"/>
+      <c r="W11" s="18"/>
+      <c r="X11" s="18"/>
+      <c r="Y11" s="18"/>
+      <c r="Z11" s="18"/>
+      <c r="AA11" s="18"/>
+      <c r="AB11" s="17"/>
+      <c r="AC11" s="5"/>
+      <c r="AD11" s="5"/>
+      <c r="AE11" s="5"/>
+      <c r="AF11" s="5"/>
+    </row>
+    <row r="12" spans="2:32" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B12">
+        <v>8</v>
+      </c>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="5"/>
+      <c r="M12" s="5"/>
+      <c r="N12" s="18"/>
+      <c r="O12" s="18"/>
+      <c r="P12" s="5"/>
+      <c r="Q12" s="18"/>
+      <c r="R12" s="5"/>
+      <c r="S12" s="5"/>
+      <c r="T12" s="5"/>
+      <c r="U12" s="5"/>
+      <c r="V12" s="18"/>
+      <c r="W12" s="18"/>
+      <c r="X12" s="5"/>
+      <c r="Y12" s="5"/>
+      <c r="Z12" s="18"/>
+      <c r="AA12" s="18"/>
+      <c r="AB12" s="5"/>
+      <c r="AC12" s="5"/>
+      <c r="AD12" s="5"/>
+      <c r="AE12" s="5"/>
+      <c r="AF12" s="5"/>
+    </row>
+    <row r="13" spans="2:32" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B13">
+        <v>9</v>
+      </c>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="5"/>
+      <c r="M13" s="5"/>
+      <c r="N13" s="18"/>
+      <c r="O13" s="18"/>
+      <c r="P13" s="18"/>
+      <c r="Q13" s="18"/>
+      <c r="R13" s="5"/>
+      <c r="S13" s="5"/>
+      <c r="T13" s="5"/>
+      <c r="U13" s="18"/>
+      <c r="V13" s="18"/>
+      <c r="W13" s="5"/>
+      <c r="X13" s="5"/>
+      <c r="Y13" s="5"/>
+      <c r="Z13" s="5"/>
+      <c r="AA13" s="5"/>
+      <c r="AB13" s="5"/>
+      <c r="AC13" s="5"/>
+      <c r="AD13" s="5"/>
+      <c r="AE13" s="5"/>
+      <c r="AF13" s="5"/>
+    </row>
+    <row r="14" spans="2:32" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B14">
+        <v>10</v>
+      </c>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="5"/>
+      <c r="L14" s="5"/>
+      <c r="M14" s="5"/>
+      <c r="N14" s="5"/>
+      <c r="O14" s="18"/>
+      <c r="P14" s="18"/>
+      <c r="Q14" s="5"/>
+      <c r="R14" s="5"/>
+      <c r="S14" s="5"/>
+      <c r="T14" s="18"/>
+      <c r="U14" s="18"/>
+      <c r="V14" s="5"/>
+      <c r="W14" s="5"/>
+      <c r="X14" s="5"/>
+      <c r="Y14" s="5"/>
+      <c r="Z14" s="5"/>
+      <c r="AA14" s="5"/>
+      <c r="AB14" s="5"/>
+      <c r="AC14" s="5"/>
+      <c r="AD14" s="5"/>
+      <c r="AE14" s="5"/>
+      <c r="AF14" s="5"/>
+    </row>
+    <row r="15" spans="2:32" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B15">
+        <v>11</v>
+      </c>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="5"/>
+      <c r="L15" s="5"/>
+      <c r="M15" s="5"/>
+      <c r="N15" s="5"/>
+      <c r="O15" s="18"/>
+      <c r="P15" s="18"/>
+      <c r="Q15" s="18"/>
+      <c r="R15" s="18"/>
+      <c r="S15" s="18"/>
+      <c r="T15" s="18"/>
+      <c r="U15" s="5"/>
+      <c r="V15" s="5"/>
+      <c r="W15" s="5"/>
+      <c r="X15" s="5"/>
+      <c r="Y15" s="5"/>
+      <c r="Z15" s="5"/>
+      <c r="AA15" s="5"/>
+      <c r="AB15" s="5"/>
+      <c r="AC15" s="5"/>
+      <c r="AD15" s="5"/>
+      <c r="AE15" s="5"/>
+      <c r="AF15" s="5"/>
+    </row>
+    <row r="16" spans="2:32" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B16">
+        <v>12</v>
+      </c>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="5"/>
+      <c r="L16" s="5"/>
+      <c r="M16" s="5"/>
+      <c r="N16" s="5"/>
+      <c r="O16" s="18"/>
+      <c r="P16" s="18"/>
+      <c r="Q16" s="18"/>
+      <c r="R16" s="5"/>
+      <c r="S16" s="5"/>
+      <c r="T16" s="5"/>
+      <c r="U16" s="5"/>
+      <c r="V16" s="5"/>
+      <c r="W16" s="5"/>
+      <c r="X16" s="5"/>
+      <c r="Y16" s="5"/>
+      <c r="Z16" s="5"/>
+      <c r="AA16" s="5"/>
+      <c r="AB16" s="5"/>
+      <c r="AC16" s="5"/>
+      <c r="AD16" s="5"/>
+      <c r="AE16" s="5"/>
+      <c r="AF16" s="5"/>
+    </row>
+    <row r="17" spans="2:32" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B17">
+        <v>13</v>
+      </c>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="5"/>
+      <c r="K17" s="5"/>
+      <c r="L17" s="5"/>
+      <c r="M17" s="5"/>
+      <c r="N17" s="5"/>
+      <c r="O17" s="18"/>
+      <c r="P17" s="18"/>
+      <c r="Q17" s="5"/>
+      <c r="R17" s="5"/>
+      <c r="S17" s="5"/>
+      <c r="T17" s="5"/>
+      <c r="U17" s="5"/>
+      <c r="V17" s="5"/>
+      <c r="W17" s="5"/>
+      <c r="X17" s="5"/>
+      <c r="Y17" s="5"/>
+      <c r="Z17" s="5"/>
+      <c r="AA17" s="5"/>
+      <c r="AB17" s="5"/>
+      <c r="AC17" s="5"/>
+      <c r="AD17" s="5"/>
+      <c r="AE17" s="5"/>
+      <c r="AF17" s="5"/>
+    </row>
+    <row r="18" spans="2:32" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B18">
+        <v>14</v>
+      </c>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="5"/>
+      <c r="L18" s="5"/>
+      <c r="M18" s="5"/>
+      <c r="N18" s="5"/>
+      <c r="O18" s="17"/>
+      <c r="P18" s="17"/>
+      <c r="Q18" s="5"/>
+      <c r="R18" s="5"/>
+      <c r="S18" s="5"/>
+      <c r="T18" s="5"/>
+      <c r="U18" s="5"/>
+      <c r="V18" s="5"/>
+      <c r="W18" s="5"/>
+      <c r="X18" s="5"/>
+      <c r="Y18" s="5"/>
+      <c r="Z18" s="5"/>
+      <c r="AA18" s="5"/>
+      <c r="AB18" s="5"/>
+      <c r="AC18" s="5"/>
+      <c r="AD18" s="5"/>
+      <c r="AE18" s="5"/>
+      <c r="AF18" s="5"/>
+    </row>
+    <row r="19" spans="2:32" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B19">
+        <v>15</v>
+      </c>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="5"/>
+      <c r="K19" s="5"/>
+      <c r="L19" s="5"/>
+      <c r="M19" s="5"/>
+      <c r="N19" s="5"/>
+      <c r="O19" s="17"/>
+      <c r="P19" s="17"/>
+      <c r="Q19" s="5"/>
+      <c r="R19" s="5"/>
+      <c r="S19" s="18"/>
+      <c r="T19" s="18"/>
+      <c r="U19" s="18"/>
+      <c r="V19" s="5"/>
+      <c r="W19" s="5"/>
+      <c r="X19" s="5"/>
+      <c r="Y19" s="5"/>
+      <c r="Z19" s="5"/>
+      <c r="AA19" s="5"/>
+      <c r="AB19" s="5"/>
+      <c r="AC19" s="5"/>
+      <c r="AD19" s="5"/>
+      <c r="AE19" s="5"/>
+      <c r="AF19" s="5"/>
+    </row>
+    <row r="20" spans="2:32" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B20">
+        <v>16</v>
+      </c>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
+      <c r="I20" s="5"/>
+      <c r="J20" s="5"/>
+      <c r="K20" s="5"/>
+      <c r="L20" s="5"/>
+      <c r="M20" s="5"/>
+      <c r="N20" s="5"/>
+      <c r="O20" s="17"/>
+      <c r="P20" s="17"/>
+      <c r="Q20" s="5"/>
+      <c r="R20" s="18"/>
+      <c r="S20" s="18"/>
+      <c r="T20" s="5"/>
+      <c r="U20" s="18"/>
+      <c r="V20" s="5"/>
+      <c r="W20" s="5"/>
+      <c r="X20" s="5"/>
+      <c r="Y20" s="5"/>
+      <c r="Z20" s="5"/>
+      <c r="AA20" s="5"/>
+      <c r="AB20" s="5"/>
+      <c r="AC20" s="5"/>
+      <c r="AD20" s="5"/>
+      <c r="AE20" s="5"/>
+      <c r="AF20" s="5"/>
+    </row>
+    <row r="21" spans="2:32" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B21">
+        <v>17</v>
+      </c>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="5"/>
+      <c r="J21" s="5"/>
+      <c r="K21" s="5"/>
+      <c r="L21" s="5"/>
+      <c r="M21" s="5"/>
+      <c r="N21" s="5"/>
+      <c r="O21" s="17"/>
+      <c r="P21" s="17"/>
+      <c r="Q21" s="18"/>
+      <c r="R21" s="18"/>
+      <c r="S21" s="5"/>
+      <c r="T21" s="5"/>
+      <c r="U21" s="5"/>
+      <c r="V21" s="5"/>
+      <c r="W21" s="5"/>
+      <c r="X21" s="5"/>
+      <c r="Y21" s="5"/>
+      <c r="Z21" s="5"/>
+      <c r="AA21" s="5"/>
+      <c r="AB21" s="5"/>
+      <c r="AC21" s="5"/>
+      <c r="AD21" s="5"/>
+      <c r="AE21" s="5"/>
+      <c r="AF21" s="5"/>
+    </row>
+    <row r="22" spans="2:32" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B22">
+        <v>18</v>
+      </c>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="5"/>
+      <c r="J22" s="5"/>
+      <c r="K22" s="5"/>
+      <c r="L22" s="5"/>
+      <c r="M22" s="5"/>
+      <c r="N22" s="5"/>
+      <c r="O22" s="17"/>
+      <c r="P22" s="17"/>
+      <c r="Q22" s="18"/>
+      <c r="R22" s="5"/>
+      <c r="S22" s="5"/>
+      <c r="T22" s="5"/>
+      <c r="U22" s="5"/>
+      <c r="V22" s="5"/>
+      <c r="W22" s="5"/>
+      <c r="X22" s="5"/>
+      <c r="Y22" s="5"/>
+      <c r="Z22" s="5"/>
+      <c r="AA22" s="5"/>
+      <c r="AB22" s="5"/>
+      <c r="AC22" s="5"/>
+      <c r="AD22" s="5"/>
+      <c r="AE22" s="5"/>
+      <c r="AF22" s="5"/>
+    </row>
+    <row r="23" spans="2:32" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B23">
+        <v>19</v>
+      </c>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="5"/>
+      <c r="J23" s="5"/>
+      <c r="K23" s="5"/>
+      <c r="L23" s="5"/>
+      <c r="M23" s="5"/>
+      <c r="N23" s="5"/>
+      <c r="O23" s="17"/>
+      <c r="P23" s="17"/>
+      <c r="Q23" s="5"/>
+      <c r="R23" s="5"/>
+      <c r="S23" s="5"/>
+      <c r="T23" s="5"/>
+      <c r="U23" s="5"/>
+      <c r="V23" s="5"/>
+      <c r="W23" s="5"/>
+      <c r="X23" s="5"/>
+      <c r="Y23" s="5"/>
+      <c r="Z23" s="5"/>
+      <c r="AA23" s="5"/>
+      <c r="AB23" s="5"/>
+      <c r="AC23" s="5"/>
+      <c r="AD23" s="5"/>
+      <c r="AE23" s="5"/>
+      <c r="AF23" s="5"/>
+    </row>
+    <row r="24" spans="2:32" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B24">
+        <v>20</v>
+      </c>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="5"/>
+      <c r="J24" s="5"/>
+      <c r="K24" s="5"/>
+      <c r="L24" s="5"/>
+      <c r="M24" s="5"/>
+      <c r="N24" s="5"/>
+      <c r="O24" s="17"/>
+      <c r="P24" s="17"/>
+      <c r="Q24" s="5"/>
+      <c r="R24" s="5"/>
+      <c r="S24" s="5"/>
+      <c r="T24" s="5"/>
+      <c r="U24" s="5"/>
+      <c r="V24" s="5"/>
+      <c r="W24" s="5"/>
+      <c r="X24" s="5"/>
+      <c r="Y24" s="5"/>
+      <c r="Z24" s="5"/>
+      <c r="AA24" s="5"/>
+      <c r="AB24" s="5"/>
+      <c r="AC24" s="5"/>
+      <c r="AD24" s="5"/>
+      <c r="AE24" s="5"/>
+      <c r="AF24" s="5"/>
+    </row>
+    <row r="25" spans="2:32" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B25">
+        <v>21</v>
+      </c>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="18"/>
+      <c r="H25" s="18"/>
+      <c r="I25" s="18"/>
+      <c r="J25" s="18"/>
+      <c r="K25" s="18"/>
+      <c r="L25" s="5"/>
+      <c r="M25" s="5"/>
+      <c r="N25" s="5"/>
+      <c r="O25" s="17"/>
+      <c r="P25" s="17"/>
+      <c r="Q25" s="5"/>
+      <c r="R25" s="5"/>
+      <c r="S25" s="5"/>
+      <c r="T25" s="5"/>
+      <c r="U25" s="5"/>
+      <c r="V25" s="5"/>
+      <c r="W25" s="5"/>
+      <c r="X25" s="5"/>
+      <c r="Y25" s="5"/>
+      <c r="Z25" s="5"/>
+      <c r="AA25" s="5"/>
+      <c r="AB25" s="5"/>
+      <c r="AC25" s="5"/>
+      <c r="AD25" s="5"/>
+      <c r="AE25" s="5"/>
+      <c r="AF25" s="5"/>
+    </row>
+    <row r="26" spans="2:32" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B26">
+        <v>22</v>
+      </c>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="5"/>
+      <c r="I26" s="5"/>
+      <c r="J26" s="5"/>
+      <c r="K26" s="5"/>
+      <c r="L26" s="18"/>
+      <c r="M26" s="18"/>
+      <c r="N26" s="18"/>
+      <c r="O26" s="17"/>
+      <c r="P26" s="17"/>
+      <c r="Q26" s="16"/>
+      <c r="R26" s="16"/>
+      <c r="S26" s="16"/>
+      <c r="T26" s="16"/>
+      <c r="U26" s="16"/>
+      <c r="V26" s="16"/>
+      <c r="W26" s="16"/>
+      <c r="X26" s="16"/>
+      <c r="Y26" s="16"/>
+      <c r="Z26" s="16"/>
+      <c r="AA26" s="16"/>
+      <c r="AB26" s="5"/>
+      <c r="AC26" s="5"/>
+      <c r="AD26" s="5"/>
+      <c r="AE26" s="5"/>
+      <c r="AF26" s="5"/>
+    </row>
+    <row r="27" spans="2:32" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B27">
+        <v>23</v>
+      </c>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="5"/>
+      <c r="H27" s="5"/>
+      <c r="I27" s="5"/>
+      <c r="J27" s="5"/>
+      <c r="K27" s="5"/>
+      <c r="L27" s="5"/>
+      <c r="M27" s="5"/>
+      <c r="N27" s="18"/>
+      <c r="O27" s="17"/>
+      <c r="P27" s="17"/>
+      <c r="Q27" s="5"/>
+      <c r="R27" s="5"/>
+      <c r="S27" s="5"/>
+      <c r="T27" s="5"/>
+      <c r="U27" s="5"/>
+      <c r="V27" s="5"/>
+      <c r="W27" s="5"/>
+      <c r="X27" s="5"/>
+      <c r="Y27" s="5"/>
+      <c r="Z27" s="5"/>
+      <c r="AA27" s="5"/>
+      <c r="AB27" s="5"/>
+      <c r="AC27" s="5"/>
+      <c r="AD27" s="5"/>
+      <c r="AE27" s="5"/>
+      <c r="AF27" s="5"/>
+    </row>
+    <row r="28" spans="2:32" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B28">
+        <v>24</v>
+      </c>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="5"/>
+      <c r="H28" s="5"/>
+      <c r="I28" s="5"/>
+      <c r="J28" s="5"/>
+      <c r="K28" s="5"/>
+      <c r="L28" s="5"/>
+      <c r="M28" s="5"/>
+      <c r="N28" s="18"/>
+      <c r="O28" s="17"/>
+      <c r="P28" s="17"/>
+      <c r="Q28" s="5"/>
+      <c r="R28" s="5"/>
+      <c r="S28" s="5"/>
+      <c r="T28" s="5"/>
+      <c r="U28" s="5"/>
+      <c r="V28" s="5"/>
+      <c r="W28" s="5"/>
+      <c r="X28" s="5"/>
+      <c r="Y28" s="5"/>
+      <c r="Z28" s="5"/>
+      <c r="AA28" s="5"/>
+      <c r="AB28" s="5"/>
+      <c r="AC28" s="5"/>
+      <c r="AD28" s="5"/>
+      <c r="AE28" s="5"/>
+      <c r="AF28" s="5"/>
+    </row>
+    <row r="29" spans="2:32" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B29">
+        <v>25</v>
+      </c>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="5"/>
+      <c r="H29" s="5"/>
+      <c r="I29" s="5"/>
+      <c r="J29" s="5"/>
+      <c r="K29" s="5"/>
+      <c r="L29" s="5"/>
+      <c r="M29" s="5"/>
+      <c r="N29" s="18"/>
+      <c r="O29" s="17"/>
+      <c r="P29" s="17"/>
+      <c r="Q29" s="5"/>
+      <c r="R29" s="5"/>
+      <c r="S29" s="5"/>
+      <c r="T29" s="5"/>
+      <c r="U29" s="5"/>
+      <c r="V29" s="5"/>
+      <c r="W29" s="5"/>
+      <c r="X29" s="5"/>
+      <c r="Y29" s="5"/>
+      <c r="Z29" s="5"/>
+      <c r="AA29" s="5"/>
+      <c r="AB29" s="5"/>
+      <c r="AC29" s="5"/>
+      <c r="AD29" s="5"/>
+      <c r="AE29" s="5"/>
+      <c r="AF29" s="5"/>
+    </row>
+    <row r="30" spans="2:32" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B30">
+        <v>26</v>
+      </c>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="5"/>
+      <c r="G30" s="5"/>
+      <c r="H30" s="5"/>
+      <c r="I30" s="5"/>
+      <c r="J30" s="5"/>
+      <c r="K30" s="5"/>
+      <c r="L30" s="5"/>
+      <c r="M30" s="5"/>
+      <c r="N30" s="18"/>
+      <c r="O30" s="17"/>
+      <c r="P30" s="17"/>
+      <c r="Q30" s="5"/>
+      <c r="R30" s="5"/>
+      <c r="S30" s="5"/>
+      <c r="T30" s="5"/>
+      <c r="U30" s="5"/>
+      <c r="V30" s="5"/>
+      <c r="W30" s="5"/>
+      <c r="X30" s="5"/>
+      <c r="Y30" s="5"/>
+      <c r="Z30" s="5"/>
+      <c r="AA30" s="5"/>
+      <c r="AB30" s="5"/>
+      <c r="AC30" s="5"/>
+      <c r="AD30" s="5"/>
+      <c r="AE30" s="5"/>
+      <c r="AF30" s="5"/>
+    </row>
+    <row r="31" spans="2:32" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B31">
+        <v>27</v>
+      </c>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="5"/>
+      <c r="G31" s="5"/>
+      <c r="H31" s="5"/>
+      <c r="I31" s="5"/>
+      <c r="J31" s="5"/>
+      <c r="K31" s="5"/>
+      <c r="L31" s="5"/>
+      <c r="M31" s="5"/>
+      <c r="N31" s="18"/>
+      <c r="O31" s="17"/>
+      <c r="P31" s="17"/>
+      <c r="Q31" s="5"/>
+      <c r="R31" s="5"/>
+      <c r="S31" s="5"/>
+      <c r="T31" s="5"/>
+      <c r="U31" s="5"/>
+      <c r="V31" s="5"/>
+      <c r="W31" s="5"/>
+      <c r="X31" s="5"/>
+      <c r="Y31" s="5"/>
+      <c r="Z31" s="5"/>
+      <c r="AA31" s="5"/>
+      <c r="AB31" s="5"/>
+      <c r="AC31" s="5"/>
+      <c r="AD31" s="5"/>
+      <c r="AE31" s="5"/>
+      <c r="AF31" s="5"/>
+    </row>
+    <row r="32" spans="2:32" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B32">
+        <v>28</v>
+      </c>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="5"/>
+      <c r="H32" s="5"/>
+      <c r="I32" s="5"/>
+      <c r="J32" s="5"/>
+      <c r="K32" s="5"/>
+      <c r="L32" s="5"/>
+      <c r="M32" s="5"/>
+      <c r="N32" s="18"/>
+      <c r="O32" s="17"/>
+      <c r="P32" s="17"/>
+      <c r="Q32" s="5"/>
+      <c r="R32" s="5"/>
+      <c r="S32" s="5"/>
+      <c r="T32" s="5"/>
+      <c r="U32" s="5"/>
+      <c r="V32" s="5"/>
+      <c r="W32" s="5"/>
+      <c r="X32" s="5"/>
+      <c r="Y32" s="5"/>
+      <c r="Z32" s="5"/>
+      <c r="AA32" s="5"/>
+      <c r="AB32" s="5"/>
+      <c r="AC32" s="5"/>
+      <c r="AD32" s="5"/>
+      <c r="AE32" s="5"/>
+      <c r="AF32" s="5"/>
+    </row>
+    <row r="33" spans="2:32" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B33">
+        <v>29</v>
+      </c>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="5"/>
+      <c r="G33" s="5"/>
+      <c r="H33" s="5"/>
+      <c r="I33" s="5"/>
+      <c r="J33" s="5"/>
+      <c r="K33" s="5"/>
+      <c r="L33" s="5"/>
+      <c r="M33" s="5"/>
+      <c r="N33" s="18"/>
+      <c r="O33" s="17"/>
+      <c r="P33" s="17"/>
+      <c r="Q33" s="5"/>
+      <c r="R33" s="5"/>
+      <c r="S33" s="5"/>
+      <c r="T33" s="5"/>
+      <c r="U33" s="5"/>
+      <c r="V33" s="5"/>
+      <c r="W33" s="5"/>
+      <c r="X33" s="5"/>
+      <c r="Y33" s="5"/>
+      <c r="Z33" s="5"/>
+      <c r="AA33" s="5"/>
+      <c r="AB33" s="5"/>
+      <c r="AC33" s="5"/>
+      <c r="AD33" s="5"/>
+      <c r="AE33" s="5"/>
+      <c r="AF33" s="5"/>
+    </row>
+    <row r="34" spans="2:32" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="35" spans="2:32" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="36" spans="2:32" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="37" spans="2:32" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="38" spans="2:32" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="39" spans="2:32" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="40" spans="2:32" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="41" spans="2:32" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
New river design. New program to load rivers directly from Excel
</commit_message>
<xml_diff>
--- a/Game/River designs.xlsx
+++ b/Game/River designs.xlsx
@@ -28,19 +28,22 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="3">
   <si>
     <t>Fc</t>
   </si>
   <si>
     <t>LinearDecayPollution()</t>
   </si>
+  <si>
+    <t>r</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -54,6 +57,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri (Body)"/>
     </font>
   </fonts>
   <fills count="7">
@@ -259,8 +267,8 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1137,115 +1145,116 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:AF41"/>
+  <dimension ref="A1:AD41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="AI14" sqref="AI14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S20" sqref="S20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="34" width="4.83203125" customWidth="1"/>
+    <col min="1" max="34" width="4.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:32" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="2" spans="2:32" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="3" spans="2:32" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <v>2</v>
-      </c>
-      <c r="F3">
-        <v>3</v>
-      </c>
-      <c r="G3">
-        <v>4</v>
-      </c>
-      <c r="H3">
-        <v>5</v>
-      </c>
-      <c r="I3">
-        <v>6</v>
-      </c>
-      <c r="J3">
-        <v>7</v>
-      </c>
-      <c r="K3">
-        <v>8</v>
-      </c>
-      <c r="L3">
-        <v>9</v>
-      </c>
-      <c r="M3">
-        <v>10</v>
-      </c>
-      <c r="N3">
-        <v>11</v>
-      </c>
-      <c r="O3">
-        <v>12</v>
-      </c>
-      <c r="P3">
-        <v>13</v>
-      </c>
-      <c r="Q3">
-        <v>14</v>
-      </c>
-      <c r="R3">
-        <v>15</v>
-      </c>
-      <c r="S3">
-        <v>16</v>
-      </c>
-      <c r="T3">
-        <v>17</v>
-      </c>
-      <c r="U3">
-        <v>18</v>
-      </c>
-      <c r="V3">
-        <v>19</v>
-      </c>
-      <c r="W3">
-        <v>20</v>
-      </c>
-      <c r="X3">
-        <v>21</v>
-      </c>
-      <c r="Y3">
-        <v>22</v>
-      </c>
-      <c r="Z3">
-        <v>23</v>
-      </c>
-      <c r="AA3">
-        <v>24</v>
-      </c>
-      <c r="AB3">
-        <v>25</v>
-      </c>
-      <c r="AC3">
-        <v>26</v>
-      </c>
-      <c r="AD3">
-        <v>27</v>
-      </c>
-      <c r="AE3">
-        <v>28</v>
-      </c>
-      <c r="AF3">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" spans="2:32" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4">
-        <v>0</v>
-      </c>
+    <row r="1" spans="1:30" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="5"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
+      <c r="P1" s="5"/>
+      <c r="Q1" s="5"/>
+      <c r="R1" s="5"/>
+      <c r="S1" s="5"/>
+      <c r="T1" s="5"/>
+      <c r="U1" s="5"/>
+      <c r="V1" s="5"/>
+      <c r="W1" s="5"/>
+      <c r="X1" s="5"/>
+      <c r="Y1" s="5"/>
+      <c r="Z1" s="5"/>
+      <c r="AA1" s="5"/>
+      <c r="AB1" s="5"/>
+      <c r="AC1" s="5"/>
+      <c r="AD1" s="5"/>
+    </row>
+    <row r="2" spans="1:30" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
+      <c r="Q2" s="5"/>
+      <c r="R2" s="5"/>
+      <c r="S2" s="5"/>
+      <c r="T2" s="5"/>
+      <c r="U2" s="5"/>
+      <c r="V2" s="5"/>
+      <c r="W2" s="5"/>
+      <c r="X2" s="5"/>
+      <c r="Y2" s="5"/>
+      <c r="Z2" s="5"/>
+      <c r="AA2" s="5"/>
+      <c r="AB2" s="5"/>
+      <c r="AC2" s="5"/>
+      <c r="AD2" s="5"/>
+    </row>
+    <row r="3" spans="1:30" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="5"/>
+      <c r="O3" s="5"/>
+      <c r="P3" s="5"/>
+      <c r="Q3" s="5"/>
+      <c r="R3" s="5"/>
+      <c r="S3" s="5"/>
+      <c r="T3" s="5"/>
+      <c r="U3" s="5"/>
+      <c r="V3" s="5"/>
+      <c r="W3" s="5"/>
+      <c r="X3" s="5"/>
+      <c r="Y3" s="5"/>
+      <c r="Z3" s="5"/>
+      <c r="AA3" s="5"/>
+      <c r="AB3" s="5"/>
+      <c r="AC3" s="5"/>
+      <c r="AD3" s="5"/>
+    </row>
+    <row r="4" spans="1:30" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="5"/>
+      <c r="B4" s="5"/>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
@@ -1274,13 +1283,10 @@
       <c r="AB4" s="5"/>
       <c r="AC4" s="5"/>
       <c r="AD4" s="5"/>
-      <c r="AE4" s="5"/>
-      <c r="AF4" s="5"/>
-    </row>
-    <row r="5" spans="2:32" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5">
-        <v>1</v>
-      </c>
+    </row>
+    <row r="5" spans="1:30" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
@@ -1296,7 +1302,9 @@
       <c r="O5" s="5"/>
       <c r="P5" s="5"/>
       <c r="Q5" s="5"/>
-      <c r="R5" s="5"/>
+      <c r="R5" s="17" t="s">
+        <v>2</v>
+      </c>
       <c r="S5" s="5"/>
       <c r="T5" s="5"/>
       <c r="U5" s="5"/>
@@ -1309,19 +1317,22 @@
       <c r="AB5" s="5"/>
       <c r="AC5" s="5"/>
       <c r="AD5" s="5"/>
-      <c r="AE5" s="5"/>
-      <c r="AF5" s="5"/>
-    </row>
-    <row r="6" spans="2:32" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6">
-        <v>2</v>
-      </c>
+    </row>
+    <row r="6" spans="1:30" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
+      <c r="F6" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="G6" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="H6" s="17" t="s">
+        <v>2</v>
+      </c>
       <c r="I6" s="5"/>
       <c r="J6" s="5"/>
       <c r="K6" s="5"/>
@@ -1330,7 +1341,9 @@
       <c r="N6" s="5"/>
       <c r="O6" s="5"/>
       <c r="P6" s="5"/>
-      <c r="Q6" s="5"/>
+      <c r="Q6" s="17" t="s">
+        <v>2</v>
+      </c>
       <c r="R6" s="5"/>
       <c r="S6" s="5"/>
       <c r="T6" s="5"/>
@@ -1344,27 +1357,36 @@
       <c r="AB6" s="5"/>
       <c r="AC6" s="5"/>
       <c r="AD6" s="5"/>
-      <c r="AE6" s="5"/>
-      <c r="AF6" s="5"/>
-    </row>
-    <row r="7" spans="2:32" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7">
-        <v>3</v>
-      </c>
+    </row>
+    <row r="7" spans="1:30" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="5"/>
+      <c r="B7" s="5"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="5"/>
-      <c r="L7" s="5"/>
+      <c r="H7" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="I7" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="J7" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="K7" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="L7" s="17" t="s">
+        <v>2</v>
+      </c>
       <c r="M7" s="5"/>
       <c r="N7" s="5"/>
       <c r="O7" s="5"/>
-      <c r="P7" s="5"/>
+      <c r="P7" s="17" t="s">
+        <v>2</v>
+      </c>
       <c r="Q7" s="5"/>
       <c r="R7" s="5"/>
       <c r="S7" s="5"/>
@@ -1372,90 +1394,117 @@
       <c r="U7" s="5"/>
       <c r="V7" s="5"/>
       <c r="W7" s="5"/>
-      <c r="X7" s="5"/>
+      <c r="X7" s="17" t="s">
+        <v>2</v>
+      </c>
       <c r="Y7" s="5"/>
       <c r="Z7" s="5"/>
       <c r="AA7" s="5"/>
       <c r="AB7" s="5"/>
       <c r="AC7" s="5"/>
       <c r="AD7" s="5"/>
-      <c r="AE7" s="5"/>
-      <c r="AF7" s="5"/>
-    </row>
-    <row r="8" spans="2:32" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8">
-        <v>4</v>
-      </c>
+    </row>
+    <row r="8" spans="1:30" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="18"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
       <c r="I8" s="5"/>
       <c r="J8" s="5"/>
-      <c r="K8" s="5"/>
-      <c r="L8" s="5"/>
-      <c r="M8" s="5"/>
+      <c r="K8" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="L8" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="M8" s="17" t="s">
+        <v>2</v>
+      </c>
       <c r="N8" s="5"/>
-      <c r="O8" s="5"/>
+      <c r="O8" s="17" t="s">
+        <v>2</v>
+      </c>
       <c r="P8" s="5"/>
       <c r="Q8" s="5"/>
       <c r="R8" s="5"/>
       <c r="S8" s="5"/>
-      <c r="T8" s="18"/>
-      <c r="U8" s="5"/>
-      <c r="V8" s="5"/>
-      <c r="W8" s="5"/>
-      <c r="X8" s="5"/>
-      <c r="Y8" s="5"/>
-      <c r="Z8" s="5"/>
+      <c r="T8" s="5"/>
+      <c r="U8" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="V8" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="W8" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="X8" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y8" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z8" s="18" t="s">
+        <v>2</v>
+      </c>
       <c r="AA8" s="5"/>
       <c r="AB8" s="5"/>
       <c r="AC8" s="5"/>
       <c r="AD8" s="5"/>
-      <c r="AE8" s="5"/>
-      <c r="AF8" s="5"/>
-    </row>
-    <row r="9" spans="2:32" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9">
-        <v>5</v>
-      </c>
+    </row>
+    <row r="9" spans="1:30" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
-      <c r="G9" s="18"/>
-      <c r="H9" s="18"/>
-      <c r="I9" s="18"/>
-      <c r="J9" s="18"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
       <c r="K9" s="5"/>
-      <c r="L9" s="5"/>
-      <c r="M9" s="5"/>
+      <c r="L9" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="M9" s="17" t="s">
+        <v>2</v>
+      </c>
       <c r="N9" s="5"/>
-      <c r="O9" s="5"/>
+      <c r="O9" s="17" t="s">
+        <v>2</v>
+      </c>
       <c r="P9" s="5"/>
       <c r="Q9" s="5"/>
       <c r="R9" s="5"/>
-      <c r="S9" s="18"/>
-      <c r="T9" s="5"/>
-      <c r="U9" s="5"/>
+      <c r="S9" s="5"/>
+      <c r="T9" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="U9" s="17" t="s">
+        <v>2</v>
+      </c>
       <c r="V9" s="5"/>
       <c r="W9" s="5"/>
-      <c r="X9" s="5"/>
-      <c r="Y9" s="5"/>
+      <c r="X9" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y9" s="17" t="s">
+        <v>2</v>
+      </c>
       <c r="Z9" s="5"/>
       <c r="AA9" s="5"/>
       <c r="AB9" s="5"/>
       <c r="AC9" s="5"/>
       <c r="AD9" s="5"/>
-      <c r="AE9" s="5"/>
-      <c r="AF9" s="5"/>
-    </row>
-    <row r="10" spans="2:32" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10">
-        <v>6</v>
-      </c>
+    </row>
+    <row r="10" spans="1:30" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="5"/>
+      <c r="B10" s="5"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
@@ -1463,34 +1512,43 @@
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
       <c r="I10" s="5"/>
-      <c r="J10" s="18"/>
-      <c r="K10" s="18"/>
-      <c r="L10" s="18"/>
-      <c r="M10" s="18"/>
-      <c r="N10" s="18"/>
-      <c r="O10" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="M10" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="N10" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="O10" s="17" t="s">
+        <v>2</v>
+      </c>
       <c r="P10" s="5"/>
       <c r="Q10" s="5"/>
-      <c r="R10" s="18"/>
-      <c r="S10" s="5"/>
-      <c r="T10" s="5"/>
+      <c r="R10" s="5"/>
+      <c r="S10" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="T10" s="17" t="s">
+        <v>2</v>
+      </c>
       <c r="U10" s="5"/>
       <c r="V10" s="5"/>
       <c r="W10" s="5"/>
       <c r="X10" s="5"/>
       <c r="Y10" s="5"/>
-      <c r="Z10" s="18"/>
+      <c r="Z10" s="5"/>
       <c r="AA10" s="5"/>
       <c r="AB10" s="5"/>
       <c r="AC10" s="5"/>
       <c r="AD10" s="5"/>
-      <c r="AE10" s="5"/>
-      <c r="AF10" s="5"/>
-    </row>
-    <row r="11" spans="2:32" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11">
-        <v>7</v>
-      </c>
+    </row>
+    <row r="11" spans="1:30" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="5"/>
+      <c r="B11" s="5"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
@@ -1501,31 +1559,36 @@
       <c r="J11" s="5"/>
       <c r="K11" s="5"/>
       <c r="L11" s="5"/>
-      <c r="M11" s="18"/>
-      <c r="N11" s="18"/>
-      <c r="O11" s="18"/>
+      <c r="M11" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="N11" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="O11" s="5"/>
       <c r="P11" s="5"/>
-      <c r="Q11" s="18"/>
-      <c r="R11" s="5"/>
-      <c r="S11" s="5"/>
+      <c r="Q11" s="5"/>
+      <c r="R11" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="S11" s="17" t="s">
+        <v>2</v>
+      </c>
       <c r="T11" s="5"/>
       <c r="U11" s="5"/>
       <c r="V11" s="5"/>
-      <c r="W11" s="18"/>
-      <c r="X11" s="18"/>
-      <c r="Y11" s="18"/>
-      <c r="Z11" s="18"/>
-      <c r="AA11" s="18"/>
-      <c r="AB11" s="17"/>
+      <c r="W11" s="5"/>
+      <c r="X11" s="5"/>
+      <c r="Y11" s="5"/>
+      <c r="Z11" s="5"/>
+      <c r="AA11" s="5"/>
+      <c r="AB11" s="5"/>
       <c r="AC11" s="5"/>
       <c r="AD11" s="5"/>
-      <c r="AE11" s="5"/>
-      <c r="AF11" s="5"/>
-    </row>
-    <row r="12" spans="2:32" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12">
-        <v>8</v>
-      </c>
+    </row>
+    <row r="12" spans="1:30" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="5"/>
+      <c r="B12" s="5"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
@@ -1536,31 +1599,40 @@
       <c r="J12" s="5"/>
       <c r="K12" s="5"/>
       <c r="L12" s="5"/>
-      <c r="M12" s="5"/>
-      <c r="N12" s="18"/>
-      <c r="O12" s="18"/>
-      <c r="P12" s="5"/>
-      <c r="Q12" s="18"/>
-      <c r="R12" s="5"/>
+      <c r="M12" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="N12" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="O12" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="P12" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q12" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="R12" s="17" t="s">
+        <v>2</v>
+      </c>
       <c r="S12" s="5"/>
       <c r="T12" s="5"/>
       <c r="U12" s="5"/>
-      <c r="V12" s="18"/>
-      <c r="W12" s="18"/>
+      <c r="V12" s="5"/>
+      <c r="W12" s="5"/>
       <c r="X12" s="5"/>
       <c r="Y12" s="5"/>
-      <c r="Z12" s="18"/>
-      <c r="AA12" s="18"/>
+      <c r="Z12" s="5"/>
+      <c r="AA12" s="5"/>
       <c r="AB12" s="5"/>
       <c r="AC12" s="5"/>
       <c r="AD12" s="5"/>
-      <c r="AE12" s="5"/>
-      <c r="AF12" s="5"/>
-    </row>
-    <row r="13" spans="2:32" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13">
-        <v>9</v>
-      </c>
+    </row>
+    <row r="13" spans="1:30" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="5"/>
+      <c r="B13" s="5"/>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
@@ -1571,16 +1643,22 @@
       <c r="J13" s="5"/>
       <c r="K13" s="5"/>
       <c r="L13" s="5"/>
-      <c r="M13" s="5"/>
-      <c r="N13" s="18"/>
-      <c r="O13" s="18"/>
-      <c r="P13" s="18"/>
-      <c r="Q13" s="18"/>
+      <c r="M13" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="N13" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="O13" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="P13" s="5"/>
+      <c r="Q13" s="5"/>
       <c r="R13" s="5"/>
       <c r="S13" s="5"/>
       <c r="T13" s="5"/>
-      <c r="U13" s="18"/>
-      <c r="V13" s="18"/>
+      <c r="U13" s="5"/>
+      <c r="V13" s="5"/>
       <c r="W13" s="5"/>
       <c r="X13" s="5"/>
       <c r="Y13" s="5"/>
@@ -1589,13 +1667,10 @@
       <c r="AB13" s="5"/>
       <c r="AC13" s="5"/>
       <c r="AD13" s="5"/>
-      <c r="AE13" s="5"/>
-      <c r="AF13" s="5"/>
-    </row>
-    <row r="14" spans="2:32" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14">
-        <v>10</v>
-      </c>
+    </row>
+    <row r="14" spans="1:30" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="5"/>
+      <c r="B14" s="5"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
@@ -1606,15 +1681,19 @@
       <c r="J14" s="5"/>
       <c r="K14" s="5"/>
       <c r="L14" s="5"/>
-      <c r="M14" s="5"/>
-      <c r="N14" s="5"/>
-      <c r="O14" s="18"/>
-      <c r="P14" s="18"/>
+      <c r="M14" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="N14" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="O14" s="5"/>
+      <c r="P14" s="5"/>
       <c r="Q14" s="5"/>
       <c r="R14" s="5"/>
       <c r="S14" s="5"/>
-      <c r="T14" s="18"/>
-      <c r="U14" s="18"/>
+      <c r="T14" s="5"/>
+      <c r="U14" s="5"/>
       <c r="V14" s="5"/>
       <c r="W14" s="5"/>
       <c r="X14" s="5"/>
@@ -1624,13 +1703,10 @@
       <c r="AB14" s="5"/>
       <c r="AC14" s="5"/>
       <c r="AD14" s="5"/>
-      <c r="AE14" s="5"/>
-      <c r="AF14" s="5"/>
-    </row>
-    <row r="15" spans="2:32" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15">
-        <v>11</v>
-      </c>
+    </row>
+    <row r="15" spans="1:30" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="5"/>
+      <c r="B15" s="5"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
@@ -1640,15 +1716,21 @@
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
       <c r="K15" s="5"/>
-      <c r="L15" s="5"/>
-      <c r="M15" s="5"/>
-      <c r="N15" s="5"/>
-      <c r="O15" s="18"/>
-      <c r="P15" s="18"/>
-      <c r="Q15" s="18"/>
-      <c r="R15" s="18"/>
-      <c r="S15" s="18"/>
-      <c r="T15" s="18"/>
+      <c r="L15" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="M15" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="N15" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="O15" s="5"/>
+      <c r="P15" s="5"/>
+      <c r="Q15" s="5"/>
+      <c r="R15" s="5"/>
+      <c r="S15" s="5"/>
+      <c r="T15" s="5"/>
       <c r="U15" s="5"/>
       <c r="V15" s="5"/>
       <c r="W15" s="5"/>
@@ -1659,13 +1741,10 @@
       <c r="AB15" s="5"/>
       <c r="AC15" s="5"/>
       <c r="AD15" s="5"/>
-      <c r="AE15" s="5"/>
-      <c r="AF15" s="5"/>
-    </row>
-    <row r="16" spans="2:32" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16">
-        <v>12</v>
-      </c>
+    </row>
+    <row r="16" spans="1:30" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="5"/>
+      <c r="B16" s="5"/>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
@@ -1675,12 +1754,16 @@
       <c r="I16" s="5"/>
       <c r="J16" s="5"/>
       <c r="K16" s="5"/>
-      <c r="L16" s="5"/>
-      <c r="M16" s="5"/>
+      <c r="L16" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="M16" s="17" t="s">
+        <v>2</v>
+      </c>
       <c r="N16" s="5"/>
-      <c r="O16" s="18"/>
-      <c r="P16" s="18"/>
-      <c r="Q16" s="18"/>
+      <c r="O16" s="5"/>
+      <c r="P16" s="5"/>
+      <c r="Q16" s="5"/>
       <c r="R16" s="5"/>
       <c r="S16" s="5"/>
       <c r="T16" s="5"/>
@@ -1694,13 +1777,10 @@
       <c r="AB16" s="5"/>
       <c r="AC16" s="5"/>
       <c r="AD16" s="5"/>
-      <c r="AE16" s="5"/>
-      <c r="AF16" s="5"/>
-    </row>
-    <row r="17" spans="2:32" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17">
-        <v>13</v>
-      </c>
+    </row>
+    <row r="17" spans="1:30" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="5"/>
+      <c r="B17" s="5"/>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
@@ -1710,14 +1790,26 @@
       <c r="I17" s="5"/>
       <c r="J17" s="5"/>
       <c r="K17" s="5"/>
-      <c r="L17" s="5"/>
-      <c r="M17" s="5"/>
-      <c r="N17" s="5"/>
-      <c r="O17" s="18"/>
-      <c r="P17" s="18"/>
-      <c r="Q17" s="5"/>
-      <c r="R17" s="5"/>
-      <c r="S17" s="5"/>
+      <c r="L17" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="M17" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="N17" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="O17" s="5"/>
+      <c r="P17" s="5"/>
+      <c r="Q17" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="R17" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="S17" s="17" t="s">
+        <v>2</v>
+      </c>
       <c r="T17" s="5"/>
       <c r="U17" s="5"/>
       <c r="V17" s="5"/>
@@ -1729,13 +1821,10 @@
       <c r="AB17" s="5"/>
       <c r="AC17" s="5"/>
       <c r="AD17" s="5"/>
-      <c r="AE17" s="5"/>
-      <c r="AF17" s="5"/>
-    </row>
-    <row r="18" spans="2:32" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18">
-        <v>14</v>
-      </c>
+    </row>
+    <row r="18" spans="1:30" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="5"/>
+      <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
@@ -1746,13 +1835,23 @@
       <c r="J18" s="5"/>
       <c r="K18" s="5"/>
       <c r="L18" s="5"/>
-      <c r="M18" s="5"/>
-      <c r="N18" s="5"/>
-      <c r="O18" s="17"/>
-      <c r="P18" s="17"/>
-      <c r="Q18" s="5"/>
+      <c r="M18" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="N18" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="O18" s="5"/>
+      <c r="P18" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q18" s="17" t="s">
+        <v>2</v>
+      </c>
       <c r="R18" s="5"/>
-      <c r="S18" s="5"/>
+      <c r="S18" s="17" t="s">
+        <v>2</v>
+      </c>
       <c r="T18" s="5"/>
       <c r="U18" s="5"/>
       <c r="V18" s="5"/>
@@ -1764,13 +1863,10 @@
       <c r="AB18" s="5"/>
       <c r="AC18" s="5"/>
       <c r="AD18" s="5"/>
-      <c r="AE18" s="5"/>
-      <c r="AF18" s="5"/>
-    </row>
-    <row r="19" spans="2:32" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19">
-        <v>15</v>
-      </c>
+    </row>
+    <row r="19" spans="1:30" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="5"/>
+      <c r="B19" s="5"/>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
@@ -1781,15 +1877,23 @@
       <c r="J19" s="5"/>
       <c r="K19" s="5"/>
       <c r="L19" s="5"/>
-      <c r="M19" s="5"/>
-      <c r="N19" s="5"/>
-      <c r="O19" s="17"/>
-      <c r="P19" s="17"/>
+      <c r="M19" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="N19" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="O19" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="P19" s="17" t="s">
+        <v>2</v>
+      </c>
       <c r="Q19" s="5"/>
       <c r="R19" s="5"/>
-      <c r="S19" s="18"/>
-      <c r="T19" s="18"/>
-      <c r="U19" s="18"/>
+      <c r="S19" s="5"/>
+      <c r="T19" s="5"/>
+      <c r="U19" s="5"/>
       <c r="V19" s="5"/>
       <c r="W19" s="5"/>
       <c r="X19" s="5"/>
@@ -1799,32 +1903,37 @@
       <c r="AB19" s="5"/>
       <c r="AC19" s="5"/>
       <c r="AD19" s="5"/>
-      <c r="AE19" s="5"/>
-      <c r="AF19" s="5"/>
-    </row>
-    <row r="20" spans="2:32" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20">
-        <v>16</v>
-      </c>
+    </row>
+    <row r="20" spans="1:30" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="5"/>
+      <c r="B20" s="5"/>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
+      <c r="F20" s="17" t="s">
+        <v>2</v>
+      </c>
       <c r="G20" s="5"/>
       <c r="H20" s="5"/>
       <c r="I20" s="5"/>
       <c r="J20" s="5"/>
       <c r="K20" s="5"/>
       <c r="L20" s="5"/>
-      <c r="M20" s="5"/>
-      <c r="N20" s="5"/>
-      <c r="O20" s="17"/>
-      <c r="P20" s="17"/>
+      <c r="M20" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="N20" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="O20" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="P20" s="5"/>
       <c r="Q20" s="5"/>
-      <c r="R20" s="18"/>
-      <c r="S20" s="18"/>
+      <c r="R20" s="5"/>
+      <c r="S20" s="5"/>
       <c r="T20" s="5"/>
-      <c r="U20" s="18"/>
+      <c r="U20" s="5"/>
       <c r="V20" s="5"/>
       <c r="W20" s="5"/>
       <c r="X20" s="5"/>
@@ -1834,29 +1943,32 @@
       <c r="AB20" s="5"/>
       <c r="AC20" s="5"/>
       <c r="AD20" s="5"/>
-      <c r="AE20" s="5"/>
-      <c r="AF20" s="5"/>
-    </row>
-    <row r="21" spans="2:32" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21">
-        <v>17</v>
-      </c>
+    </row>
+    <row r="21" spans="1:30" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="5"/>
+      <c r="B21" s="5"/>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
+      <c r="F21" s="17" t="s">
+        <v>2</v>
+      </c>
       <c r="G21" s="5"/>
       <c r="H21" s="5"/>
       <c r="I21" s="5"/>
       <c r="J21" s="5"/>
       <c r="K21" s="5"/>
       <c r="L21" s="5"/>
-      <c r="M21" s="5"/>
-      <c r="N21" s="5"/>
-      <c r="O21" s="17"/>
-      <c r="P21" s="17"/>
-      <c r="Q21" s="18"/>
-      <c r="R21" s="18"/>
+      <c r="M21" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="N21" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="O21" s="5"/>
+      <c r="P21" s="5"/>
+      <c r="Q21" s="5"/>
+      <c r="R21" s="5"/>
       <c r="S21" s="5"/>
       <c r="T21" s="5"/>
       <c r="U21" s="5"/>
@@ -1869,28 +1981,37 @@
       <c r="AB21" s="5"/>
       <c r="AC21" s="5"/>
       <c r="AD21" s="5"/>
-      <c r="AE21" s="5"/>
-      <c r="AF21" s="5"/>
-    </row>
-    <row r="22" spans="2:32" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B22">
-        <v>18</v>
-      </c>
+    </row>
+    <row r="22" spans="1:30" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="5"/>
+      <c r="B22" s="5"/>
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="5"/>
-      <c r="I22" s="5"/>
+      <c r="F22" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="G22" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="H22" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="I22" s="17" t="s">
+        <v>2</v>
+      </c>
       <c r="J22" s="5"/>
       <c r="K22" s="5"/>
       <c r="L22" s="5"/>
-      <c r="M22" s="5"/>
-      <c r="N22" s="5"/>
-      <c r="O22" s="17"/>
-      <c r="P22" s="17"/>
-      <c r="Q22" s="18"/>
+      <c r="M22" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="N22" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="O22" s="5"/>
+      <c r="P22" s="5"/>
+      <c r="Q22" s="5"/>
       <c r="R22" s="5"/>
       <c r="S22" s="5"/>
       <c r="T22" s="5"/>
@@ -1904,48 +2025,56 @@
       <c r="AB22" s="5"/>
       <c r="AC22" s="5"/>
       <c r="AD22" s="5"/>
-      <c r="AE22" s="5"/>
-      <c r="AF22" s="5"/>
-    </row>
-    <row r="23" spans="2:32" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B23">
-        <v>19</v>
-      </c>
+    </row>
+    <row r="23" spans="1:30" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="5"/>
+      <c r="B23" s="5"/>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
       <c r="G23" s="5"/>
       <c r="H23" s="5"/>
-      <c r="I23" s="5"/>
-      <c r="J23" s="5"/>
-      <c r="K23" s="5"/>
-      <c r="L23" s="5"/>
-      <c r="M23" s="5"/>
-      <c r="N23" s="5"/>
-      <c r="O23" s="17"/>
-      <c r="P23" s="17"/>
-      <c r="Q23" s="5"/>
-      <c r="R23" s="5"/>
-      <c r="S23" s="5"/>
-      <c r="T23" s="5"/>
-      <c r="U23" s="5"/>
-      <c r="V23" s="5"/>
-      <c r="W23" s="5"/>
-      <c r="X23" s="5"/>
-      <c r="Y23" s="5"/>
+      <c r="I23" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="J23" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="K23" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="L23" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="M23" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="N23" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="O23" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="P23" s="16"/>
+      <c r="Q23" s="16"/>
+      <c r="R23" s="16"/>
+      <c r="S23" s="16"/>
+      <c r="T23" s="16"/>
+      <c r="U23" s="16"/>
+      <c r="V23" s="16"/>
+      <c r="W23" s="16"/>
+      <c r="X23" s="16"/>
+      <c r="Y23" s="16"/>
       <c r="Z23" s="5"/>
       <c r="AA23" s="5"/>
       <c r="AB23" s="5"/>
       <c r="AC23" s="5"/>
       <c r="AD23" s="5"/>
-      <c r="AE23" s="5"/>
-      <c r="AF23" s="5"/>
-    </row>
-    <row r="24" spans="2:32" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B24">
-        <v>20</v>
-      </c>
+    </row>
+    <row r="24" spans="1:30" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="5"/>
+      <c r="B24" s="5"/>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
@@ -1957,9 +2086,13 @@
       <c r="K24" s="5"/>
       <c r="L24" s="5"/>
       <c r="M24" s="5"/>
-      <c r="N24" s="5"/>
-      <c r="O24" s="17"/>
-      <c r="P24" s="17"/>
+      <c r="N24" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="O24" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="P24" s="5"/>
       <c r="Q24" s="5"/>
       <c r="R24" s="5"/>
       <c r="S24" s="5"/>
@@ -1974,27 +2107,30 @@
       <c r="AB24" s="5"/>
       <c r="AC24" s="5"/>
       <c r="AD24" s="5"/>
-      <c r="AE24" s="5"/>
-      <c r="AF24" s="5"/>
-    </row>
-    <row r="25" spans="2:32" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B25">
-        <v>21</v>
-      </c>
+    </row>
+    <row r="25" spans="1:30" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="5"/>
+      <c r="B25" s="5"/>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
-      <c r="G25" s="18"/>
-      <c r="H25" s="18"/>
-      <c r="I25" s="18"/>
-      <c r="J25" s="18"/>
-      <c r="K25" s="18"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="5"/>
+      <c r="J25" s="5"/>
+      <c r="K25" s="5"/>
       <c r="L25" s="5"/>
       <c r="M25" s="5"/>
-      <c r="N25" s="5"/>
-      <c r="O25" s="17"/>
-      <c r="P25" s="17"/>
+      <c r="N25" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="O25" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="P25" s="17" t="s">
+        <v>2</v>
+      </c>
       <c r="Q25" s="5"/>
       <c r="R25" s="5"/>
       <c r="S25" s="5"/>
@@ -2009,13 +2145,10 @@
       <c r="AB25" s="5"/>
       <c r="AC25" s="5"/>
       <c r="AD25" s="5"/>
-      <c r="AE25" s="5"/>
-      <c r="AF25" s="5"/>
-    </row>
-    <row r="26" spans="2:32" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B26">
-        <v>22</v>
-      </c>
+    </row>
+    <row r="26" spans="1:30" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="5"/>
+      <c r="B26" s="5"/>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
       <c r="E26" s="5"/>
@@ -2025,32 +2158,35 @@
       <c r="I26" s="5"/>
       <c r="J26" s="5"/>
       <c r="K26" s="5"/>
-      <c r="L26" s="18"/>
-      <c r="M26" s="18"/>
-      <c r="N26" s="18"/>
-      <c r="O26" s="17"/>
-      <c r="P26" s="17"/>
-      <c r="Q26" s="16"/>
-      <c r="R26" s="16"/>
-      <c r="S26" s="16"/>
-      <c r="T26" s="16"/>
-      <c r="U26" s="16"/>
-      <c r="V26" s="16"/>
-      <c r="W26" s="16"/>
-      <c r="X26" s="16"/>
-      <c r="Y26" s="16"/>
-      <c r="Z26" s="16"/>
-      <c r="AA26" s="16"/>
+      <c r="L26" s="5"/>
+      <c r="M26" s="5"/>
+      <c r="N26" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="O26" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="P26" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q26" s="5"/>
+      <c r="R26" s="5"/>
+      <c r="S26" s="5"/>
+      <c r="T26" s="5"/>
+      <c r="U26" s="5"/>
+      <c r="V26" s="5"/>
+      <c r="W26" s="5"/>
+      <c r="X26" s="5"/>
+      <c r="Y26" s="5"/>
+      <c r="Z26" s="5"/>
+      <c r="AA26" s="5"/>
       <c r="AB26" s="5"/>
       <c r="AC26" s="5"/>
       <c r="AD26" s="5"/>
-      <c r="AE26" s="5"/>
-      <c r="AF26" s="5"/>
-    </row>
-    <row r="27" spans="2:32" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B27">
-        <v>23</v>
-      </c>
+    </row>
+    <row r="27" spans="1:30" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="5"/>
+      <c r="B27" s="5"/>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
@@ -2062,10 +2198,16 @@
       <c r="K27" s="5"/>
       <c r="L27" s="5"/>
       <c r="M27" s="5"/>
-      <c r="N27" s="18"/>
-      <c r="O27" s="17"/>
-      <c r="P27" s="17"/>
-      <c r="Q27" s="5"/>
+      <c r="N27" s="5"/>
+      <c r="O27" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="P27" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q27" s="17" t="s">
+        <v>2</v>
+      </c>
       <c r="R27" s="5"/>
       <c r="S27" s="5"/>
       <c r="T27" s="5"/>
@@ -2079,13 +2221,10 @@
       <c r="AB27" s="5"/>
       <c r="AC27" s="5"/>
       <c r="AD27" s="5"/>
-      <c r="AE27" s="5"/>
-      <c r="AF27" s="5"/>
-    </row>
-    <row r="28" spans="2:32" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B28">
-        <v>24</v>
-      </c>
+    </row>
+    <row r="28" spans="1:30" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="5"/>
+      <c r="B28" s="5"/>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
       <c r="E28" s="5"/>
@@ -2097,11 +2236,19 @@
       <c r="K28" s="5"/>
       <c r="L28" s="5"/>
       <c r="M28" s="5"/>
-      <c r="N28" s="18"/>
-      <c r="O28" s="17"/>
-      <c r="P28" s="17"/>
-      <c r="Q28" s="5"/>
-      <c r="R28" s="5"/>
+      <c r="N28" s="5"/>
+      <c r="O28" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="P28" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q28" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="R28" s="17" t="s">
+        <v>2</v>
+      </c>
       <c r="S28" s="5"/>
       <c r="T28" s="5"/>
       <c r="U28" s="5"/>
@@ -2114,13 +2261,10 @@
       <c r="AB28" s="5"/>
       <c r="AC28" s="5"/>
       <c r="AD28" s="5"/>
-      <c r="AE28" s="5"/>
-      <c r="AF28" s="5"/>
-    </row>
-    <row r="29" spans="2:32" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B29">
-        <v>25</v>
-      </c>
+    </row>
+    <row r="29" spans="1:30" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="5"/>
+      <c r="B29" s="5"/>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
       <c r="E29" s="5"/>
@@ -2132,11 +2276,17 @@
       <c r="K29" s="5"/>
       <c r="L29" s="5"/>
       <c r="M29" s="5"/>
-      <c r="N29" s="18"/>
-      <c r="O29" s="17"/>
-      <c r="P29" s="17"/>
-      <c r="Q29" s="5"/>
-      <c r="R29" s="5"/>
+      <c r="N29" s="5"/>
+      <c r="O29" s="5"/>
+      <c r="P29" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q29" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="R29" s="17" t="s">
+        <v>2</v>
+      </c>
       <c r="S29" s="5"/>
       <c r="T29" s="5"/>
       <c r="U29" s="5"/>
@@ -2149,13 +2299,10 @@
       <c r="AB29" s="5"/>
       <c r="AC29" s="5"/>
       <c r="AD29" s="5"/>
-      <c r="AE29" s="5"/>
-      <c r="AF29" s="5"/>
-    </row>
-    <row r="30" spans="2:32" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B30">
-        <v>26</v>
-      </c>
+    </row>
+    <row r="30" spans="1:30" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="5"/>
+      <c r="B30" s="5"/>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
       <c r="E30" s="5"/>
@@ -2167,11 +2314,17 @@
       <c r="K30" s="5"/>
       <c r="L30" s="5"/>
       <c r="M30" s="5"/>
-      <c r="N30" s="18"/>
-      <c r="O30" s="17"/>
-      <c r="P30" s="17"/>
-      <c r="Q30" s="5"/>
-      <c r="R30" s="5"/>
+      <c r="N30" s="5"/>
+      <c r="O30" s="5"/>
+      <c r="P30" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q30" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="R30" s="17" t="s">
+        <v>2</v>
+      </c>
       <c r="S30" s="5"/>
       <c r="T30" s="5"/>
       <c r="U30" s="5"/>
@@ -2184,122 +2337,18 @@
       <c r="AB30" s="5"/>
       <c r="AC30" s="5"/>
       <c r="AD30" s="5"/>
-      <c r="AE30" s="5"/>
-      <c r="AF30" s="5"/>
-    </row>
-    <row r="31" spans="2:32" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B31">
-        <v>27</v>
-      </c>
-      <c r="C31" s="5"/>
-      <c r="D31" s="5"/>
-      <c r="E31" s="5"/>
-      <c r="F31" s="5"/>
-      <c r="G31" s="5"/>
-      <c r="H31" s="5"/>
-      <c r="I31" s="5"/>
-      <c r="J31" s="5"/>
-      <c r="K31" s="5"/>
-      <c r="L31" s="5"/>
-      <c r="M31" s="5"/>
-      <c r="N31" s="18"/>
-      <c r="O31" s="17"/>
-      <c r="P31" s="17"/>
-      <c r="Q31" s="5"/>
-      <c r="R31" s="5"/>
-      <c r="S31" s="5"/>
-      <c r="T31" s="5"/>
-      <c r="U31" s="5"/>
-      <c r="V31" s="5"/>
-      <c r="W31" s="5"/>
-      <c r="X31" s="5"/>
-      <c r="Y31" s="5"/>
-      <c r="Z31" s="5"/>
-      <c r="AA31" s="5"/>
-      <c r="AB31" s="5"/>
-      <c r="AC31" s="5"/>
-      <c r="AD31" s="5"/>
-      <c r="AE31" s="5"/>
-      <c r="AF31" s="5"/>
-    </row>
-    <row r="32" spans="2:32" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B32">
-        <v>28</v>
-      </c>
-      <c r="C32" s="5"/>
-      <c r="D32" s="5"/>
-      <c r="E32" s="5"/>
-      <c r="F32" s="5"/>
-      <c r="G32" s="5"/>
-      <c r="H32" s="5"/>
-      <c r="I32" s="5"/>
-      <c r="J32" s="5"/>
-      <c r="K32" s="5"/>
-      <c r="L32" s="5"/>
-      <c r="M32" s="5"/>
-      <c r="N32" s="18"/>
-      <c r="O32" s="17"/>
-      <c r="P32" s="17"/>
-      <c r="Q32" s="5"/>
-      <c r="R32" s="5"/>
-      <c r="S32" s="5"/>
-      <c r="T32" s="5"/>
-      <c r="U32" s="5"/>
-      <c r="V32" s="5"/>
-      <c r="W32" s="5"/>
-      <c r="X32" s="5"/>
-      <c r="Y32" s="5"/>
-      <c r="Z32" s="5"/>
-      <c r="AA32" s="5"/>
-      <c r="AB32" s="5"/>
-      <c r="AC32" s="5"/>
-      <c r="AD32" s="5"/>
-      <c r="AE32" s="5"/>
-      <c r="AF32" s="5"/>
-    </row>
-    <row r="33" spans="2:32" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B33">
-        <v>29</v>
-      </c>
-      <c r="C33" s="5"/>
-      <c r="D33" s="5"/>
-      <c r="E33" s="5"/>
-      <c r="F33" s="5"/>
-      <c r="G33" s="5"/>
-      <c r="H33" s="5"/>
-      <c r="I33" s="5"/>
-      <c r="J33" s="5"/>
-      <c r="K33" s="5"/>
-      <c r="L33" s="5"/>
-      <c r="M33" s="5"/>
-      <c r="N33" s="18"/>
-      <c r="O33" s="17"/>
-      <c r="P33" s="17"/>
-      <c r="Q33" s="5"/>
-      <c r="R33" s="5"/>
-      <c r="S33" s="5"/>
-      <c r="T33" s="5"/>
-      <c r="U33" s="5"/>
-      <c r="V33" s="5"/>
-      <c r="W33" s="5"/>
-      <c r="X33" s="5"/>
-      <c r="Y33" s="5"/>
-      <c r="Z33" s="5"/>
-      <c r="AA33" s="5"/>
-      <c r="AB33" s="5"/>
-      <c r="AC33" s="5"/>
-      <c r="AD33" s="5"/>
-      <c r="AE33" s="5"/>
-      <c r="AF33" s="5"/>
-    </row>
-    <row r="34" spans="2:32" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="35" spans="2:32" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="36" spans="2:32" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="37" spans="2:32" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="38" spans="2:32" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="39" spans="2:32" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="40" spans="2:32" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="41" spans="2:32" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
+    </row>
+    <row r="31" spans="1:30" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:30" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="33" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="34" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="35" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="36" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="37" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="38" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="39" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="40" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="41" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
map design for initialize with all LU in place
</commit_message>
<xml_diff>
--- a/Game/River designs.xlsx
+++ b/Game/River designs.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="22660" yWindow="460" windowWidth="28540" windowHeight="27040" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="22660" yWindow="460" windowWidth="28540" windowHeight="27040" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="River1 20x20" sheetId="1" r:id="rId1"/>
     <sheet name="River2 30x30" sheetId="2" r:id="rId2"/>
+    <sheet name="With all" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="8">
   <si>
     <t>Fc</t>
   </si>
@@ -40,6 +41,18 @@
   </si>
   <si>
     <t>f</t>
+  </si>
+  <si>
+    <t>fc</t>
+  </si>
+  <si>
+    <t>hs</t>
+  </si>
+  <si>
+    <t>fm</t>
+  </si>
+  <si>
+    <t>c</t>
   </si>
 </sst>
 </file>
@@ -1142,8 +1155,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AB28" sqref="AB28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="T12" sqref="T12:W15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1252,9 +1265,7 @@
       <c r="N3" s="5"/>
       <c r="O3" s="5"/>
       <c r="P3" s="5"/>
-      <c r="Q3" s="5" t="s">
-        <v>3</v>
-      </c>
+      <c r="Q3" s="5"/>
       <c r="R3" s="5"/>
       <c r="S3" s="5"/>
       <c r="T3" s="5"/>
@@ -1358,9 +1369,7 @@
       <c r="R5" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="S5" s="5" t="s">
-        <v>3</v>
-      </c>
+      <c r="S5" s="5"/>
       <c r="T5" s="5"/>
       <c r="U5" s="5"/>
       <c r="V5" s="5"/>
@@ -1631,9 +1640,7 @@
       </c>
       <c r="U10" s="5"/>
       <c r="V10" s="5"/>
-      <c r="W10" s="5" t="s">
-        <v>3</v>
-      </c>
+      <c r="W10" s="5"/>
       <c r="X10" s="5"/>
       <c r="Y10" s="5"/>
       <c r="Z10" s="5"/>
@@ -2340,12 +2347,8 @@
       <c r="I24" s="5"/>
       <c r="J24" s="5"/>
       <c r="K24" s="5"/>
-      <c r="L24" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="M24" s="5" t="s">
-        <v>3</v>
-      </c>
+      <c r="L24" s="5"/>
+      <c r="M24" s="5"/>
       <c r="N24" s="16" t="s">
         <v>2</v>
       </c>
@@ -2400,9 +2403,7 @@
       <c r="L25" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="M25" s="5" t="s">
-        <v>3</v>
-      </c>
+      <c r="M25" s="5"/>
       <c r="N25" s="16" t="s">
         <v>2</v>
       </c>
@@ -2440,9 +2441,7 @@
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
       <c r="E26" s="5"/>
-      <c r="F26" s="5" t="s">
-        <v>3</v>
-      </c>
+      <c r="F26" s="5"/>
       <c r="G26" s="5"/>
       <c r="H26" s="5"/>
       <c r="I26" s="5"/>
@@ -2451,9 +2450,7 @@
       <c r="L26" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="M26" s="5" t="s">
-        <v>3</v>
-      </c>
+      <c r="M26" s="5"/>
       <c r="N26" s="16" t="s">
         <v>2</v>
       </c>
@@ -2766,4 +2763,1886 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AE41"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AB14" sqref="AB14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="34" width="4.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:31" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="5"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
+      <c r="P1" s="5"/>
+      <c r="Q1" s="5"/>
+      <c r="R1" s="5"/>
+      <c r="S1" s="5"/>
+      <c r="T1" s="5"/>
+      <c r="U1" s="5"/>
+      <c r="V1" s="5"/>
+      <c r="W1" s="5"/>
+      <c r="X1" s="5"/>
+      <c r="Y1" s="5"/>
+      <c r="Z1" s="5"/>
+      <c r="AA1" s="5"/>
+      <c r="AB1" s="5"/>
+      <c r="AC1" s="5"/>
+      <c r="AD1" s="5"/>
+      <c r="AE1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:31" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="5"/>
+      <c r="B2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
+      <c r="Q2" s="5"/>
+      <c r="R2" s="5"/>
+      <c r="S2" s="5"/>
+      <c r="T2" s="5"/>
+      <c r="U2" s="5"/>
+      <c r="V2" s="5"/>
+      <c r="W2" s="5"/>
+      <c r="X2" s="5"/>
+      <c r="Y2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="Z2" s="5"/>
+      <c r="AA2" s="5"/>
+      <c r="AB2" s="5"/>
+      <c r="AC2" s="5"/>
+      <c r="AD2" s="5"/>
+      <c r="AE2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="5"/>
+      <c r="B3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="5"/>
+      <c r="O3" s="5"/>
+      <c r="P3" s="5"/>
+      <c r="Q3" s="5"/>
+      <c r="R3" s="5"/>
+      <c r="S3" s="5"/>
+      <c r="T3" s="5"/>
+      <c r="U3" s="5"/>
+      <c r="V3" s="5"/>
+      <c r="W3" s="5"/>
+      <c r="X3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="Y3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="Z3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="AA3" s="5"/>
+      <c r="AB3" s="5"/>
+      <c r="AC3" s="5"/>
+      <c r="AD3" s="5"/>
+      <c r="AE3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:31" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="5"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="5"/>
+      <c r="O4" s="5"/>
+      <c r="P4" s="5"/>
+      <c r="Q4" s="5"/>
+      <c r="R4" s="5"/>
+      <c r="S4" s="5"/>
+      <c r="T4" s="5"/>
+      <c r="U4" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="V4" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="W4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="X4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="Y4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="Z4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="AA4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="AB4" s="5"/>
+      <c r="AC4" s="5"/>
+      <c r="AD4" s="5"/>
+      <c r="AE4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:31" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="5"/>
+      <c r="O5" s="5"/>
+      <c r="P5" s="5"/>
+      <c r="Q5" s="5"/>
+      <c r="R5" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="S5" s="5"/>
+      <c r="T5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="U5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="V5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="W5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="X5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="Y5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="Z5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="AA5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="AB5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="AC5" s="5"/>
+      <c r="AD5" s="5"/>
+      <c r="AE5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:31" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="5"/>
+      <c r="B6" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" s="5"/>
+      <c r="F6" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="G6" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="H6" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5"/>
+      <c r="N6" s="5"/>
+      <c r="O6" s="5"/>
+      <c r="P6" s="5"/>
+      <c r="Q6" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="R6" s="5"/>
+      <c r="S6" s="5"/>
+      <c r="T6" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="U6" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="V6" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="W6" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="X6" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="Y6" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="Z6" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA6" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="AB6" s="5"/>
+      <c r="AC6" s="5"/>
+      <c r="AD6" s="5"/>
+      <c r="AE6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:31" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="5"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="I7" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="J7" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="K7" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="L7" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="M7" s="5"/>
+      <c r="N7" s="5"/>
+      <c r="O7" s="5"/>
+      <c r="P7" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q7" s="5"/>
+      <c r="R7" s="5"/>
+      <c r="S7" s="5"/>
+      <c r="T7" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="U7" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="V7" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="W7" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="X7" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y7" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="Z7" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA7" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="AB7" s="5"/>
+      <c r="AC7" s="5"/>
+      <c r="AD7" s="5"/>
+      <c r="AE7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:31" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="K8" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="L8" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="M8" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="N8" s="5"/>
+      <c r="O8" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="P8" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q8" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="R8" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="S8" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="T8" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="U8" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="V8" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="W8" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="X8" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y8" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z8" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA8" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="AB8" s="5"/>
+      <c r="AC8" s="5"/>
+      <c r="AD8" s="5"/>
+      <c r="AE8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:31" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="K9" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="L9" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="M9" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="N9" s="5"/>
+      <c r="O9" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="P9" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q9" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="R9" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="S9" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="T9" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="U9" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="V9" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="W9" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="X9" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y9" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z9" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA9" s="5"/>
+      <c r="AB9" s="5"/>
+      <c r="AC9" s="5"/>
+      <c r="AD9" s="5"/>
+      <c r="AE9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:31" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="5"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="L10" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="M10" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="N10" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="O10" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="P10" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q10" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="R10" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="S10" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="T10" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="U10" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="V10" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="W10" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="X10" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y10" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="Z10" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA10" s="5"/>
+      <c r="AB10" s="5"/>
+      <c r="AC10" s="5"/>
+      <c r="AD10" s="5"/>
+      <c r="AE10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:31" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="5"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="L11" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="M11" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="N11" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="O11" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="P11" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q11" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="R11" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="S11" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="T11" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="U11" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="V11" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="W11" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="X11" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y11" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="Z11" s="5"/>
+      <c r="AA11" s="5"/>
+      <c r="AB11" s="5"/>
+      <c r="AC11" s="5"/>
+      <c r="AD11" s="5"/>
+      <c r="AE11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:31" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="5"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H12" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="K12" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="L12" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="M12" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="N12" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="O12" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="P12" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q12" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="R12" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="S12" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="T12" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="U12" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="V12" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="W12" s="5"/>
+      <c r="X12" s="5"/>
+      <c r="Y12" s="5"/>
+      <c r="Z12" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="AA12" s="5"/>
+      <c r="AB12" s="5"/>
+      <c r="AC12" s="5"/>
+      <c r="AD12" s="5"/>
+      <c r="AE12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:31" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="5"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="K13" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="L13" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="M13" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="N13" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="O13" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="P13" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q13" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="R13" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="S13" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="T13" s="5"/>
+      <c r="U13" s="5"/>
+      <c r="V13" s="5"/>
+      <c r="W13" s="5"/>
+      <c r="X13" s="5"/>
+      <c r="Y13" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="Z13" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="AA13" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="AB13" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="AC13" s="5"/>
+      <c r="AD13" s="5"/>
+      <c r="AE13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:31" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="5"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="I14" s="5"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="5"/>
+      <c r="L14" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="M14" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="N14" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="O14" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="P14" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q14" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="R14" s="5"/>
+      <c r="S14" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="T14" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="U14" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="V14" s="5"/>
+      <c r="W14" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="X14" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y14" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z14" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="AA14" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="AB14" s="5"/>
+      <c r="AC14" s="5"/>
+      <c r="AD14" s="5"/>
+      <c r="AE14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:31" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="5"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="L15" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="M15" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="N15" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="O15" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="P15" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q15" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="R15" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="S15" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="T15" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="U15" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="V15" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="W15" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="X15" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y15" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z15" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA15" s="5"/>
+      <c r="AB15" s="5"/>
+      <c r="AC15" s="5"/>
+      <c r="AD15" s="5"/>
+      <c r="AE15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:31" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="5"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="K16" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="L16" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="M16" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="N16" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="O16" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="P16" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q16" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="R16" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="S16" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="T16" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="U16" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="V16" s="5"/>
+      <c r="W16" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="X16" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y16" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z16" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="AA16" s="5"/>
+      <c r="AB16" s="5"/>
+      <c r="AC16" s="5"/>
+      <c r="AD16" s="5"/>
+      <c r="AE16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:31" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="5"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="K17" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="L17" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="M17" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="N17" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="O17" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="P17" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q17" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="R17" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="S17" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="T17" s="5"/>
+      <c r="U17" s="5"/>
+      <c r="V17" s="5"/>
+      <c r="W17" s="5"/>
+      <c r="X17" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="Y17" s="5"/>
+      <c r="Z17" s="5"/>
+      <c r="AA17" s="5"/>
+      <c r="AB17" s="5"/>
+      <c r="AC17" s="5"/>
+      <c r="AD17" s="5"/>
+      <c r="AE17">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:31" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="5"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="H18" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="I18" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="J18" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="K18" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="L18" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="M18" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="N18" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="O18" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="P18" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q18" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="R18" s="5"/>
+      <c r="S18" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="T18" s="5"/>
+      <c r="U18" s="5"/>
+      <c r="V18" s="5"/>
+      <c r="W18" s="5"/>
+      <c r="X18" s="5"/>
+      <c r="Y18" s="5"/>
+      <c r="Z18" s="5"/>
+      <c r="AA18" s="5"/>
+      <c r="AB18" s="5"/>
+      <c r="AC18" s="5"/>
+      <c r="AD18" s="5"/>
+      <c r="AE18">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:31" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="5"/>
+      <c r="B19" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="H19" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="I19" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="J19" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="K19" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="L19" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="M19" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="N19" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="O19" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="P19" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q19" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="R19" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="S19" s="5"/>
+      <c r="T19" s="5"/>
+      <c r="U19" s="5"/>
+      <c r="V19" s="5"/>
+      <c r="W19" s="5"/>
+      <c r="X19" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="Y19" s="5"/>
+      <c r="Z19" s="5"/>
+      <c r="AA19" s="5"/>
+      <c r="AB19" s="5"/>
+      <c r="AC19" s="5"/>
+      <c r="AD19" s="5"/>
+      <c r="AE19">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:31" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="5"/>
+      <c r="B20" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E20" s="5"/>
+      <c r="F20" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="I20" s="5"/>
+      <c r="J20" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="K20" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="L20" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="M20" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="N20" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="O20" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="P20" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q20" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="R20" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="S20" s="5"/>
+      <c r="T20" s="5"/>
+      <c r="U20" s="5"/>
+      <c r="V20" s="5"/>
+      <c r="W20" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="X20" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="Y20" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="Z20" s="5"/>
+      <c r="AA20" s="5"/>
+      <c r="AB20" s="5"/>
+      <c r="AC20" s="5"/>
+      <c r="AD20" s="5"/>
+      <c r="AE20">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:31" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="5"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="5"/>
+      <c r="J21" s="5"/>
+      <c r="K21" s="5"/>
+      <c r="L21" s="5"/>
+      <c r="M21" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="N21" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="O21" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="P21" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q21" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="R21" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="S21" s="5"/>
+      <c r="T21" s="5"/>
+      <c r="U21" s="5"/>
+      <c r="V21" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="W21" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="X21" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="Y21" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="Z21" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="AA21" s="5"/>
+      <c r="AB21" s="5"/>
+      <c r="AC21" s="5"/>
+      <c r="AD21" s="5"/>
+      <c r="AE21">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:31" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="5"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="G22" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="H22" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="I22" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="J22" s="5"/>
+      <c r="K22" s="5"/>
+      <c r="L22" s="5"/>
+      <c r="M22" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="N22" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="O22" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="P22" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q22" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="R22" s="5"/>
+      <c r="S22" s="5"/>
+      <c r="T22" s="5"/>
+      <c r="U22" s="5"/>
+      <c r="V22" s="5"/>
+      <c r="W22" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="X22" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="Y22" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="Z22" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="AA22" s="5"/>
+      <c r="AB22" s="5"/>
+      <c r="AC22" s="5"/>
+      <c r="AD22" s="5"/>
+      <c r="AE22">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:31" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="5"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="J23" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="K23" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="L23" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="M23" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="N23" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="O23" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="P23" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q23" s="5"/>
+      <c r="R23" s="5"/>
+      <c r="S23" s="5"/>
+      <c r="T23" s="5"/>
+      <c r="U23" s="5"/>
+      <c r="V23" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="W23" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="X23" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="Y23" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="Z23" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="AA23" s="5"/>
+      <c r="AB23" s="5"/>
+      <c r="AC23" s="5"/>
+      <c r="AD23" s="5"/>
+      <c r="AE23">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:31" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="5"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="5"/>
+      <c r="J24" s="5"/>
+      <c r="K24" s="5"/>
+      <c r="L24" s="5"/>
+      <c r="M24" s="5"/>
+      <c r="N24" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="O24" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="P24" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q24" s="5"/>
+      <c r="R24" s="5"/>
+      <c r="S24" s="5"/>
+      <c r="T24" s="5"/>
+      <c r="U24" s="5"/>
+      <c r="V24" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="W24" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="X24" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="Y24" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="Z24" s="5"/>
+      <c r="AA24" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="AB24" s="5"/>
+      <c r="AC24" s="5"/>
+      <c r="AD24" s="5"/>
+      <c r="AE24">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:31" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="5"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="5"/>
+      <c r="J25" s="5"/>
+      <c r="K25" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="L25" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="M25" s="5"/>
+      <c r="N25" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="O25" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="P25" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q25" s="5"/>
+      <c r="R25" s="5"/>
+      <c r="S25" s="5"/>
+      <c r="T25" s="5"/>
+      <c r="U25" s="5"/>
+      <c r="V25" s="5"/>
+      <c r="W25" s="5"/>
+      <c r="X25" s="5"/>
+      <c r="Y25" s="5"/>
+      <c r="Z25" s="5"/>
+      <c r="AA25" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="AB25" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="AC25" s="5"/>
+      <c r="AD25" s="5"/>
+      <c r="AE25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:31" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="5"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="5"/>
+      <c r="I26" s="5"/>
+      <c r="J26" s="5"/>
+      <c r="K26" s="5"/>
+      <c r="L26" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="M26" s="5"/>
+      <c r="N26" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="O26" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="P26" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q26" s="5"/>
+      <c r="R26" s="5"/>
+      <c r="S26" s="5"/>
+      <c r="T26" s="5"/>
+      <c r="U26" s="5"/>
+      <c r="V26" s="5"/>
+      <c r="W26" s="5"/>
+      <c r="X26" s="5"/>
+      <c r="Y26" s="5"/>
+      <c r="Z26" s="5"/>
+      <c r="AA26" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="AB26" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="AC26" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="AD26" s="5"/>
+      <c r="AE26">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:31" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="5"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="5"/>
+      <c r="H27" s="5"/>
+      <c r="I27" s="5"/>
+      <c r="J27" s="5"/>
+      <c r="K27" s="5"/>
+      <c r="L27" s="5"/>
+      <c r="M27" s="5"/>
+      <c r="N27" s="5"/>
+      <c r="O27" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="P27" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q27" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="R27" s="5"/>
+      <c r="S27" s="5"/>
+      <c r="T27" s="5"/>
+      <c r="U27" s="5"/>
+      <c r="V27" s="5"/>
+      <c r="W27" s="5"/>
+      <c r="X27" s="5"/>
+      <c r="Y27" s="5"/>
+      <c r="Z27" s="5"/>
+      <c r="AA27" s="5"/>
+      <c r="AB27" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="AC27" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="AD27" s="5"/>
+      <c r="AE27">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:31" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="5"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="5"/>
+      <c r="H28" s="5"/>
+      <c r="I28" s="5"/>
+      <c r="J28" s="5"/>
+      <c r="K28" s="5"/>
+      <c r="L28" s="5"/>
+      <c r="M28" s="5"/>
+      <c r="N28" s="5"/>
+      <c r="O28" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="P28" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q28" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="R28" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="S28" s="5"/>
+      <c r="T28" s="5"/>
+      <c r="U28" s="5"/>
+      <c r="V28" s="5"/>
+      <c r="W28" s="5"/>
+      <c r="X28" s="5"/>
+      <c r="Y28" s="5"/>
+      <c r="Z28" s="5"/>
+      <c r="AA28" s="5"/>
+      <c r="AB28" s="5"/>
+      <c r="AC28" s="5"/>
+      <c r="AD28" s="5"/>
+      <c r="AE28">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:31" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="5"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="5"/>
+      <c r="H29" s="5"/>
+      <c r="I29" s="5"/>
+      <c r="J29" s="5"/>
+      <c r="K29" s="5"/>
+      <c r="L29" s="5"/>
+      <c r="M29" s="5"/>
+      <c r="N29" s="5"/>
+      <c r="O29" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="P29" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q29" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="R29" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="S29" s="5"/>
+      <c r="T29" s="5"/>
+      <c r="U29" s="5"/>
+      <c r="V29" s="5"/>
+      <c r="W29" s="5"/>
+      <c r="X29" s="5"/>
+      <c r="Y29" s="5"/>
+      <c r="Z29" s="5"/>
+      <c r="AA29" s="5"/>
+      <c r="AB29" s="5"/>
+      <c r="AC29" s="5"/>
+      <c r="AD29" s="5"/>
+      <c r="AE29">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:31" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="5"/>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="5"/>
+      <c r="G30" s="5"/>
+      <c r="H30" s="5"/>
+      <c r="I30" s="5"/>
+      <c r="J30" s="5"/>
+      <c r="K30" s="5"/>
+      <c r="L30" s="5"/>
+      <c r="M30" s="5"/>
+      <c r="N30" s="5"/>
+      <c r="O30" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="P30" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q30" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="R30" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="S30" s="5"/>
+      <c r="T30" s="5"/>
+      <c r="U30" s="5"/>
+      <c r="V30" s="5"/>
+      <c r="W30" s="5"/>
+      <c r="X30" s="5"/>
+      <c r="Y30" s="5"/>
+      <c r="Z30" s="5"/>
+      <c r="AA30" s="5"/>
+      <c r="AB30" s="5"/>
+      <c r="AC30" s="5"/>
+      <c r="AD30" s="5"/>
+      <c r="AE30">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:31" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>0</v>
+      </c>
+      <c r="B31">
+        <v>1</v>
+      </c>
+      <c r="C31">
+        <v>2</v>
+      </c>
+      <c r="D31">
+        <v>3</v>
+      </c>
+      <c r="E31">
+        <v>4</v>
+      </c>
+      <c r="F31">
+        <v>5</v>
+      </c>
+      <c r="G31">
+        <v>6</v>
+      </c>
+      <c r="H31">
+        <v>7</v>
+      </c>
+      <c r="I31">
+        <v>8</v>
+      </c>
+      <c r="J31">
+        <v>9</v>
+      </c>
+      <c r="K31">
+        <v>10</v>
+      </c>
+      <c r="L31">
+        <v>11</v>
+      </c>
+      <c r="M31">
+        <v>12</v>
+      </c>
+      <c r="N31">
+        <v>13</v>
+      </c>
+      <c r="O31">
+        <v>14</v>
+      </c>
+      <c r="P31">
+        <v>15</v>
+      </c>
+      <c r="Q31">
+        <v>16</v>
+      </c>
+      <c r="R31">
+        <v>17</v>
+      </c>
+      <c r="S31">
+        <v>18</v>
+      </c>
+      <c r="T31">
+        <v>19</v>
+      </c>
+      <c r="U31">
+        <v>20</v>
+      </c>
+      <c r="V31">
+        <v>21</v>
+      </c>
+      <c r="W31">
+        <v>22</v>
+      </c>
+      <c r="X31">
+        <v>23</v>
+      </c>
+      <c r="Y31">
+        <v>24</v>
+      </c>
+      <c r="Z31">
+        <v>25</v>
+      </c>
+      <c r="AA31">
+        <v>26</v>
+      </c>
+      <c r="AB31">
+        <v>27</v>
+      </c>
+      <c r="AC31">
+        <v>28</v>
+      </c>
+      <c r="AD31">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="32" spans="1:31" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="33" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="34" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="35" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="36" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="37" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="38" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="39" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="40" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="41" ht="29" customHeight="1" x14ac:dyDescent="0.2"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>